<commit_message>
docs market & support links copy from dev
</commit_message>
<xml_diff>
--- a/docs/_sites/bakemaster_docs_links_table.xlsx
+++ b/docs/_sites/bakemaster_docs_links_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kempl\AppData\Roaming\Blender Foundation\Blender\3.2\scripts\addons\bakemaster\docs\_sites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Projects\Code\Blender\BakeMaster 2022\backup\BakeMaster-Blender-Addon-Dev\docs\_sites\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="93">
   <si>
     <t>license</t>
   </si>
@@ -297,6 +297,12 @@
   </si>
   <si>
     <t>https://github.com/KirilStrezikozin/BakeMaster-Blender-Addon/issues/new/choose</t>
+  </si>
+  <si>
+    <t>https://blendermarket.com/products/bakemaster</t>
+  </si>
+  <si>
+    <t>https://paypal.me/kemplerart</t>
   </si>
 </sst>
 </file>
@@ -655,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,19 +733,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -946,7 +940,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>61</v>
       </c>
@@ -954,7 +948,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>62</v>
       </c>
@@ -962,7 +956,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>65</v>
       </c>
@@ -970,7 +964,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>67</v>
       </c>
@@ -978,7 +972,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>70</v>
       </c>
@@ -986,7 +980,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>71</v>
       </c>
@@ -994,7 +988,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>73</v>
       </c>
@@ -1002,7 +996,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>74</v>
       </c>
@@ -1010,7 +1004,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>77</v>
       </c>
@@ -1018,7 +1012,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>79</v>
       </c>
@@ -1026,7 +1020,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>81</v>
       </c>
@@ -1034,7 +1028,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>83</v>
       </c>
@@ -1042,26 +1036,21 @@
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C45" t="s">
-        <v>85</v>
-      </c>
-      <c r="D45" t="s">
-        <v>64</v>
+      <c r="B45" s="5" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B22" r:id="rId1" location="bake-settings-panel"/>
     <hyperlink ref="B23" r:id="rId2" location="bake-instruction"/>
+    <hyperlink ref="B45" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>